<commit_message>
1st. Delivery: Initial version which works.
</commit_message>
<xml_diff>
--- a/ButecoCalc/Exemplo.xlsx
+++ b/ButecoCalc/Exemplo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19110" windowHeight="8430" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>cerveja</t>
   </si>
@@ -169,9 +169,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -190,6 +187,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -504,16 +504,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="15.75">
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" spans="2:15">
       <c r="C5" s="2" t="s">
@@ -522,7 +522,7 @@
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -549,10 +549,10 @@
       <c r="M5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -566,7 +566,7 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <f>D6*C6</f>
         <v>50</v>
       </c>
@@ -590,11 +590,11 @@
       <c r="M6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <f>COUNTIF(F6:M6,"x")</f>
         <v>6</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="8">
         <f>E6/N6</f>
         <v>8.3333333333333339</v>
       </c>
@@ -609,7 +609,7 @@
       <c r="D7" s="1">
         <v>18</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f t="shared" ref="E7:E9" si="0">D7*C7</f>
         <v>18</v>
       </c>
@@ -627,11 +627,11 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <f t="shared" ref="N7:N9" si="1">COUNTIF(F7:M7,"x")</f>
         <v>3</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="8">
         <f t="shared" ref="O7:O9" si="2">E7/N7</f>
         <v>6</v>
       </c>
@@ -646,7 +646,7 @@
       <c r="D8" s="1">
         <v>13</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -662,11 +662,11 @@
       <c r="M8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="8">
         <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
@@ -681,7 +681,7 @@
       <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -699,29 +699,29 @@
       <c r="M9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="8">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:15">
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f>SUM(E6:E9)*(1+$C$13/100)</f>
         <v>115.50000000000001</v>
       </c>
     </row>
     <row r="11" spans="2:15">
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <f>SUM(E6:E9)</f>
         <v>105</v>
       </c>
@@ -730,90 +730,90 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:15" ht="35.25" customHeight="1">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <f>(E6/N6+E7/N7)*(1+$C$13/100)</f>
         <v>15.766666666666669</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f>(E6/N6+E7/N7)*(1+$C$13/100)</f>
         <v>15.766666666666669</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <f>(E6/N6+E7/N7)*(1+$C$13/100)</f>
         <v>15.766666666666669</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <f>(E9/N9)*(1+$C$13/100)</f>
         <v>8.8000000000000007</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <f>(E9/N9)*(1+$C$13/100)</f>
         <v>8.8000000000000007</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="8">
         <f>(E6/N6)*(1+$C$13/100)</f>
         <v>9.1666666666666679</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <f>(E6/N6+E8/N8)*(1+$C$13/100)</f>
         <v>16.31666666666667</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="8">
         <f>(E6/N6+E8/N8+E9/N9)*(1+$C$13/100)</f>
         <v>25.116666666666671</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="8">
         <f>SUM(F13:M13)</f>
         <v>115.50000000000003</v>
       </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="2:15" ht="35.25" customHeight="1">
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <f>(E6/N6+E7/N7)</f>
         <v>14.333333333333334</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f>(E6/N6+E7/N7)</f>
         <v>14.333333333333334</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <f>(E6/N6+E7/N7)</f>
         <v>14.333333333333334</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <f>(E9/N9)</f>
         <v>8</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <f>(E9/N9)</f>
         <v>8</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="8">
         <f>(E6/N6)</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <f>(E6/N6+E8/N8)</f>
         <v>14.833333333333334</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="8">
         <f>(E6/N6+E8/N8+E9/N9)</f>
         <v>22.833333333333336</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="8">
         <f>SUM(F14:M14)</f>
         <v>105</v>
       </c>
@@ -830,12 +830,219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B4:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10" ht="15.75">
+      <c r="F4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6">
+        <f>D6*C6</f>
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="7">
+        <f>COUNTIF(F6:H6,"x")</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="8">
+        <f>E6/I6</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" ref="E7:E8" si="0">D7*C7</f>
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="7">
+        <f>COUNTIF(F7:H7,"x")</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="8">
+        <f>E7/I7</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="7">
+        <f>COUNTIF(F8:H8,"x")</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="8">
+        <f>E8/I8</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6">
+        <f>SUM(E6:E8)*(1+$C$12/100)</f>
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6">
+        <f>SUM(E6:E8)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" ht="45">
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="8">
+        <f>(E6/I6+E7/I7)*(1+$C$12/100)</f>
+        <v>28.233333333333338</v>
+      </c>
+      <c r="G12" s="8">
+        <f>(E6/I6+E7/I7+E8/I8)*(1+$C$12/100)</f>
+        <v>41.433333333333344</v>
+      </c>
+      <c r="H12" s="8">
+        <f>(E6/I6+E8/I8)*(1+$C$12/100)</f>
+        <v>31.533333333333339</v>
+      </c>
+      <c r="I12" s="8">
+        <f>SUM(F12:H12)</f>
+        <v>101.20000000000002</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" ht="60" customHeight="1">
+      <c r="E13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="8">
+        <f>(E6/I6+E7/I7)</f>
+        <v>25.666666666666668</v>
+      </c>
+      <c r="G13" s="8">
+        <f>(E6/I6+E7/I7+E8/I8)</f>
+        <v>37.666666666666671</v>
+      </c>
+      <c r="H13" s="8">
+        <f>(E6/I6+E8/I8)</f>
+        <v>28.666666666666668</v>
+      </c>
+      <c r="I13" s="8">
+        <f>SUM(F13:H13)</f>
+        <v>92.000000000000014</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>